<commit_message>
Auto commit 16-05-2025 14:10:32.35
</commit_message>
<xml_diff>
--- a/Templates.xlsx
+++ b/Templates.xlsx
@@ -23,131 +23,131 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Borewell Developing Charges</t>
+  </si>
+  <si>
+    <t>Supply Fitting of ISI UPVC Pipe 40mm dia</t>
+  </si>
+  <si>
+    <t>Supply Fitting of Nylon Rope 14mm thick</t>
+  </si>
+  <si>
+    <t>Pump erection charge upto 3hp</t>
+  </si>
+  <si>
+    <t>Supply fitting of NRV 40mm</t>
+  </si>
+  <si>
+    <t>Supply Fitting of SS Adaptor 40mm dia</t>
+  </si>
+  <si>
+    <t>Fabrication and Installation of Well Protection Cover</t>
+  </si>
+  <si>
+    <t>Fabrication and Installation of Metallic pump house 1.2 x 0.9 x 2m</t>
+  </si>
+  <si>
+    <t>Fabrication and Installation of Panel board Single phase</t>
+  </si>
+  <si>
+    <t>Fabrication and Installation of Iron Structure 4m for 3000 ltr water tank</t>
+  </si>
+  <si>
+    <t>Supply fitting of ISI PVC Water Tank</t>
+  </si>
+  <si>
+    <t>Tank connector 50mm</t>
+  </si>
+  <si>
+    <t>Tank connector 40mm</t>
+  </si>
+  <si>
+    <t>Supply fitting of PVC ball valve 50mm</t>
+  </si>
+  <si>
+    <t>Supply fitting of PVC ball valve 40mm</t>
+  </si>
+  <si>
+    <t>Providing and fixing ISI PVC Pipes includes jointing of pipes with one step PVC solvent cement, trenching, refilling &amp; testing of joints complete as per direction of Engineer in Charge 50mm 10kg/cm2.</t>
+  </si>
+  <si>
+    <t>Providing and fixing ISI PVC Pipes includes jointing of pipes with one step PVC solvent cement, trenching, refilling &amp; testing of joints complete as per direction of Engineer in Charge 40mm 10kg/cm2.</t>
+  </si>
+  <si>
+    <t>Providing and fixing ISI PVC Pipes includes jointing of pipes with one step PVC solvent cement, trenching, refilling &amp; testing of joints complete as per direction of Engineer in Charge 32mm 10kg/cm2.</t>
+  </si>
+  <si>
+    <t>Providing and fixing ISI PVC Pipes includes jointing of pipes with one step PVC solvent cement, trenching, refilling &amp; testing of joints complete as per direction of Engineer in Charge 25mm 10kg/cm2.</t>
+  </si>
+  <si>
+    <t>Fabrication and Installation of Individual Hydrants with tap</t>
+  </si>
+  <si>
+    <t>Trenching for pipe laying</t>
+  </si>
+  <si>
+    <t>Concrete Cutting for pipe laying in m3</t>
+  </si>
+  <si>
+    <t>Providing and laying in position cement concrete Filling 1:2:4 in m3</t>
+  </si>
+  <si>
+    <t>Supply of Compressor Pump 1.5hp single phase ISI</t>
+  </si>
+  <si>
+    <t>Compressor Pump Fitting charge</t>
+  </si>
+  <si>
+    <t>GI pipe including providing, fitting, conveyance etc (With Trenching) 25mm pipe</t>
+  </si>
+  <si>
+    <t>Supply Fitting of HDPE ISI Pipe w/o data 20mm dia</t>
+  </si>
+  <si>
+    <t>Supply Fitting of ISI UPVC Pipe 32mm dia</t>
+  </si>
+  <si>
+    <t>Supply fitting of GI Union 32mm</t>
+  </si>
+  <si>
+    <t>Supply fitting of GI Bend 32mm</t>
+  </si>
+  <si>
+    <t>Fabrication and Installation of Metallic pump cover 1 x 0.8 x 0.9m</t>
+  </si>
+  <si>
+    <t>Supply Fitting of Submersible Pump Single Phase - 1.5hp 18 stage 107-30m head ISI</t>
+  </si>
+  <si>
+    <t>Supply Fitting of Submersible 3 Core Cable ISI 4mm</t>
+  </si>
+  <si>
     <t>Earth work in excavation by mechanical means (Hydraulic excavator) /manual means in foundation trenches or drains (not exceeding 1.5 m in width or 10 sqm on plan), including dressing of sides and ramming of bottoms, lift up to 1.5 m, including getting out the excavated soil and disposal of surplus excavated soil as directed, within a lead of 50 m.
-All kinds of soil (PRICE Code: 2.8.1)</t>
+All kinds of soil (Code: 2.8.1)</t>
+  </si>
+  <si>
+    <t>Providing and laying in position cement concrete of specified grade excluding the cost of centering and shuttering - All work up to plinth level:
+1:2:4 (cement : 2 coarse sand : 4 graded stone aggregate 20mm nominal size) (Code: 4.1.3)</t>
+  </si>
+  <si>
+    <t>Providing and laying in position specified grade of reinforced cement concrete, excluding the cost of centering, shuttering, finishing and reinforcement - All work up to plinth level:
+1:2:4 ( 1 cement : 2 coarse sand : 4 graded stone aggregate 20mm nominal size) (Code: 5.1.3)</t>
   </si>
   <si>
     <t>Steel reinforcement for R.C.C work including straightening, cutting, bending, placing in position and binding all complete upto plinth level
-Mild steel and Medium Tensile steel bars (PRICE Code: 5.22.1)</t>
-  </si>
-  <si>
-    <t>Structural steel work in single section, fixed with or without connecting plate, including cutting, hoisting, fixing in position and applying a priming coat of approved steel primer all complete. (PRICE Code: 10.1)</t>
-  </si>
-  <si>
-    <t>Providing and fixing bolts including nuts and washers complete. (PRICE Code: 10.2)</t>
-  </si>
-  <si>
-    <t>Item Name</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Borewell Developing Charges</t>
-  </si>
-  <si>
-    <t>Supply Fitting of ISI UPVC Pipe 40mm dia</t>
-  </si>
-  <si>
-    <t>Supply Fitting of Nylon Rope 14mm thick</t>
-  </si>
-  <si>
-    <t>Pump erection charge upto 3hp</t>
-  </si>
-  <si>
-    <t>Supply fitting of NRV 40mm</t>
-  </si>
-  <si>
-    <t>Supply Fitting of SS Adaptor 40mm dia</t>
-  </si>
-  <si>
-    <t>Fabrication and Installation of Well Protection Cover</t>
-  </si>
-  <si>
-    <t>Fabrication and Installation of Metallic pump house 1.2 x 0.9 x 2m</t>
-  </si>
-  <si>
-    <t>Fabrication and Installation of Panel board Single phase</t>
-  </si>
-  <si>
-    <t>Fabrication and Installation of Iron Structure 4m for 3000 ltr water tank</t>
-  </si>
-  <si>
-    <t>Supply fitting of ISI PVC Water Tank</t>
-  </si>
-  <si>
-    <t>Tank connector 50mm</t>
-  </si>
-  <si>
-    <t>Tank connector 40mm</t>
-  </si>
-  <si>
-    <t>Supply fitting of PVC ball valve 50mm</t>
-  </si>
-  <si>
-    <t>Supply fitting of PVC ball valve 40mm</t>
-  </si>
-  <si>
-    <t>Providing and fixing ISI PVC Pipes includes jointing of pipes with one step PVC solvent cement, trenching, refilling &amp; testing of joints complete as per direction of Engineer in Charge 50mm 10kg/cm2.</t>
-  </si>
-  <si>
-    <t>Providing and fixing ISI PVC Pipes includes jointing of pipes with one step PVC solvent cement, trenching, refilling &amp; testing of joints complete as per direction of Engineer in Charge 40mm 10kg/cm2.</t>
-  </si>
-  <si>
-    <t>Providing and fixing ISI PVC Pipes includes jointing of pipes with one step PVC solvent cement, trenching, refilling &amp; testing of joints complete as per direction of Engineer in Charge 32mm 10kg/cm2.</t>
-  </si>
-  <si>
-    <t>Providing and fixing ISI PVC Pipes includes jointing of pipes with one step PVC solvent cement, trenching, refilling &amp; testing of joints complete as per direction of Engineer in Charge 25mm 10kg/cm2.</t>
-  </si>
-  <si>
-    <t>Fabrication and Installation of Individual Hydrants with tap</t>
-  </si>
-  <si>
-    <t>Trenching for pipe laying</t>
-  </si>
-  <si>
-    <t>Concrete Cutting for pipe laying in m3</t>
-  </si>
-  <si>
-    <t>Providing and laying in position cement concrete Filling 1:2:4 in m3</t>
-  </si>
-  <si>
-    <t>Supply of Compressor Pump 1.5hp single phase ISI</t>
-  </si>
-  <si>
-    <t>Compressor Pump Fitting charge</t>
-  </si>
-  <si>
-    <t>GI pipe including providing, fitting, conveyance etc (With Trenching) 25mm pipe</t>
-  </si>
-  <si>
-    <t>Supply Fitting of HDPE ISI Pipe w/o data 20mm dia</t>
-  </si>
-  <si>
-    <t>Supply Fitting of ISI UPVC Pipe 32mm dia</t>
-  </si>
-  <si>
-    <t>Supply fitting of GI Union 32mm</t>
-  </si>
-  <si>
-    <t>Supply fitting of GI Bend 32mm</t>
-  </si>
-  <si>
-    <t>Fabrication and Installation of Metallic pump cover 1 x 0.8 x 0.9m</t>
-  </si>
-  <si>
-    <t>Supply Fitting of Submersible Pump Single Phase - 1.5hp 18 stage 107-30m head ISI</t>
-  </si>
-  <si>
-    <t>Supply Fitting of Submersible 3 Core Cable ISI 4mm</t>
-  </si>
-  <si>
-    <t>Providing and laying in position cement concrete of specified grade excluding the cost of centering and shuttering - All work up to plinth level:
-1:2:4 (cement : 2 coarse sand : 4 graded stone aggregate 20mm nominal size) (PRICE Code: 4.1.3)</t>
-  </si>
-  <si>
-    <t>Providing and laying in position specified grade of reinforced cement concrete, excluding the cost of centering, shuttering, finishing and reinforcement - All work up to plinth level:
-1:2:4 ( 1 cement : 2 coarse sand : 4 graded stone aggregate 20mm nominal size) (PRICE Code: 5.1.3)</t>
+Mild steel and Medium Tensile steel bars (Code: 5.22.1)</t>
+  </si>
+  <si>
+    <t>Structural steel work in single section, fixed with or without connecting plate, including cutting, hoisting, fixing in position and applying a priming coat of approved steel primer all complete. (Code: 10.1)</t>
+  </si>
+  <si>
+    <t>Providing and fixing bolts including nuts and washers complete. (Code: 10.2)</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,15 +494,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="4" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="6" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -571,15 +571,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>80</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>85</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2">
         <v>85</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>3000</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="18" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="19" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>50</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="20" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>50</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="21" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>50</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="22" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
         <v>50</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>10</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>100</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="25" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
         <v>4</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="26" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>4</v>
@@ -798,15 +798,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4">
         <v>15</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4">
         <v>50</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4">
         <v>60</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B10" s="4">
         <v>65</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B11" s="4">
         <v>20</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
@@ -918,7 +918,7 @@
     </row>
     <row r="16" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="18" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B19" s="4">
         <v>3000</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22" s="4">
         <v>1</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="23" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B23" s="4">
         <v>100</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="24" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4">
         <v>100</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="25" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25" s="4">
         <v>100</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="26" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B26" s="4">
         <v>100</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="27" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B27" s="4">
         <v>10</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B28" s="4">
         <v>250</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="29" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B29" s="4">
         <v>6</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="30" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B30" s="4">
         <v>6</v>

</xml_diff>

<commit_message>
Auto commit 22-05-2025 17:22:58.72
</commit_message>
<xml_diff>
--- a/Templates.xlsx
+++ b/Templates.xlsx
@@ -147,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -155,44 +155,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,7 +440,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -477,221 +451,219 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="2"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="116" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="2">
         <v>3000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="116" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="2">
         <v>4</v>
       </c>
     </row>
@@ -705,252 +677,252 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="2" width="8.7265625" style="3"/>
+    <col min="3" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="3">
         <v>3000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="3">
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="3">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit 24-05-2025  9:25:05.10
</commit_message>
<xml_diff>
--- a/Templates.xlsx
+++ b/Templates.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Core i5 GAMING\Desktop\estimate-drafter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DC056E28-6082-474E-9404-6924CAB617B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E857EAE-18DB-4F30-B4A9-71880B2BB8F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="180" windowWidth="9855" windowHeight="7215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="180" windowWidth="9855" windowHeight="7215" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MWSS with Submersible Pump" sheetId="2" r:id="rId1"/>
     <sheet name="MWSS with Compressor Pump" sheetId="3" r:id="rId2"/>
+    <sheet name="110 mm BWC" sheetId="4" r:id="rId3"/>
+    <sheet name="150 mm BWC" sheetId="5" r:id="rId4"/>
+    <sheet name="150 mm TWC" sheetId="6" r:id="rId5"/>
+    <sheet name="200 mm TWC" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>Item Name</t>
   </si>
@@ -130,6 +134,57 @@
   </si>
   <si>
     <t>GI Bend 32 mm (Code: GWD128)</t>
+  </si>
+  <si>
+    <t>110mm (4.5") Borewell Drilling (Code: GWD248)</t>
+  </si>
+  <si>
+    <t>Supplying, assembling, lowering and fixing in vertical position in Borewell, PVC 140 mm 6 Kg/cm2 well casing pipe of required dia, conforming to IS : 4985:2000, including required hire and labour charges, fittings &amp; accessories etc. all complete, for all depths, as per direction of Engineer- in- Charge. (Code: GWD007)</t>
+  </si>
+  <si>
+    <t>PVC End cap 140 mm (Code: GWD065)</t>
+  </si>
+  <si>
+    <t>150mm (6") Borewell Drilling (Code: GWD249)</t>
+  </si>
+  <si>
+    <t>Supplying, assembling, lowering and fixing in vertical position in Borewell, PVC 180mm 10 Kg/cm2 well casing pipe of required dia, conforming to IS : 4985:2000, including required hire and labour charges, fittings &amp; accessories etc. all complete, for all depths, as per direction of Engineer- in- Charge. (Code: GWD017)</t>
+  </si>
+  <si>
+    <t>PVC End Cap 180 mm (Code: GWD067)</t>
+  </si>
+  <si>
+    <t>150mm (6") Tubewell Drilling (Code: GWD250)</t>
+  </si>
+  <si>
+    <t>Supplying, assembling, lowering and fixing in vertical position in bore well, unplasticized PVC medium well casing (CM) pipe of required dia, conforming to IS : 12818, including required hire and labour charges, fittings &amp; accessories etc. all complete, for all depths, as per direction of Engineer- in- Charge. 150 mm nominal size dia (Code: 23.3.2)</t>
+  </si>
+  <si>
+    <t>Supplying, assembling, lowering and fixing in vertical position in bore well unplasticized PVC medium well screen (RMS) pipes with ribs, conforming to IS: 12818, including hire &amp; labour charges, fittings &amp; accessories etc. all complete, for all depths, as per direction of Engineer - in-charge 150 mm nominal size dia (Code: 23.4.2)</t>
+  </si>
+  <si>
+    <t>Providing and fixing Bail plug / Bottom plug of required dia to the bottom of pipe assembly of tubewell as per IS : 2800 (part I). 150 mm dia (Code: 23.15.2)</t>
+  </si>
+  <si>
+    <t>150 mm MS end cap (7747) Basic Rate (Code: GWD024)</t>
+  </si>
+  <si>
+    <t>Tubewell Drilling over 150mm (6") (Code: GWD251)</t>
+  </si>
+  <si>
+    <t>Supplying, assembling, lowering and fixing in vertical position in bore well, unplasticized PVC medium well casing (CM) pipe of required dia, conforming to IS : 12818, including required hire and labour charges, fittings &amp; accessories etc. all complete, for all depths, as per direction of Engineer- in- Charge. 200 mm nominal size dia (Code: 23.3.3)</t>
+  </si>
+  <si>
+    <t>Supplying, assembling, lowering and fixing in vertical position in bore well unplasticized PVC medium well screen (RMS) pipes with ribs, conforming to IS: 12818, including hire &amp; labour charges, fittings &amp; accessories etc. all complete, for all depths, as per direction of Engineer - in-charge 200 mm nominal size dia (Code: 23.4.3)</t>
+  </si>
+  <si>
+    <t>Providing and fixing Bail plug / Bottom plug of required dia to the bottom of pipe assembly of tubewell as per IS : 2800 (part I). 200 mm dia (Code: 23.15.3)</t>
+  </si>
+  <si>
+    <t>200 mm MS end cap (7748) Basic Rate (Code: GWD020)</t>
+  </si>
+  <si>
+    <t>MS Casing pipe 450 mm dia, 6 mm thickness (Code: GWD203)</t>
   </si>
 </sst>
 </file>
@@ -453,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,4 +988,241 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283C56C8-5101-4528-9234-DFAFA8B3C182}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8597B7-0160-4D8F-B8C8-FDE4C5B94C30}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BB96C7-B819-4358-9077-88E63A141CF4}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52A1A6B-7BA3-45B8-8EF7-73A16298341E}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Auto commit 28-05-2025 11:31:48.36
</commit_message>
<xml_diff>
--- a/Templates.xlsx
+++ b/Templates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Core i5 GAMING\Desktop\estimate-drafter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\estimate-drafter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BF0E7E6-7B67-4AC7-AF77-58F1B1C598F2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B0F205-C920-4F98-BDB9-907A511BD51E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="180" windowWidth="9855" windowHeight="7215" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="180" windowWidth="9860" windowHeight="7220" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MWSS with Submersible Pump" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,10 @@
     <sheet name="150 mm BWC" sheetId="5" r:id="rId4"/>
     <sheet name="150 mm TWC" sheetId="6" r:id="rId5"/>
     <sheet name="200 mm TWC" sheetId="7" r:id="rId6"/>
+    <sheet name="Submersible Pump Installation" sheetId="8" r:id="rId7"/>
+    <sheet name="Compressor Pump Installation" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
   <si>
     <t>Item Name</t>
   </si>
@@ -521,12 +523,12 @@
       <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -542,7 +544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -550,7 +552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -558,7 +560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -566,7 +568,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -574,7 +576,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -582,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -590,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -598,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -606,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -614,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -622,7 +624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -630,7 +632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -638,7 +640,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -646,7 +648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -654,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -662,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -670,7 +672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -678,7 +680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -686,7 +688,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -694,7 +696,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -702,7 +704,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -710,7 +712,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -718,7 +720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -726,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -748,13 +750,13 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="3"/>
-    <col min="2" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="8.7265625" style="3"/>
+    <col min="2" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -762,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -770,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -778,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -786,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -794,7 +796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -802,7 +804,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -810,7 +812,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -818,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -826,7 +828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -834,7 +836,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -842,7 +844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -850,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -858,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -866,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -874,7 +876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -882,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -890,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -898,7 +900,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -906,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -914,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
@@ -922,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -930,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -938,7 +940,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -946,7 +948,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -954,7 +956,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -962,7 +964,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -970,7 +972,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -978,7 +980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>4</v>
       </c>
@@ -986,7 +988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -1008,9 +1010,9 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1026,7 +1028,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +1036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1056,9 +1058,9 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1074,7 +1076,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1082,7 +1084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1101,15 +1103,15 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1125,7 +1127,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1133,7 +1135,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1149,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1157,7 +1159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1175,16 +1177,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52A1A6B-7BA3-45B8-8EF7-73A16298341E}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1192,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1200,7 +1202,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1208,7 +1210,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1216,7 +1218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1224,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1232,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
@@ -1244,4 +1246,258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9A5F76-D8ED-42BD-9321-D6FD8EB33F52}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDC07DB-6CE0-44A7-A54C-721B3D36CA1E}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Auto commit 28-05-2025 11:43:03.83
</commit_message>
<xml_diff>
--- a/Templates.xlsx
+++ b/Templates.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\estimate-drafter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B0F205-C920-4F98-BDB9-907A511BD51E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239F8853-19E3-48ED-8647-7E8D7FECC7AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="180" windowWidth="9860" windowHeight="7220" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="180" windowWidth="9860" windowHeight="7220" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MWSS with Submersible Pump" sheetId="2" r:id="rId1"/>
     <sheet name="MWSS with Compressor Pump" sheetId="3" r:id="rId2"/>
-    <sheet name="110 mm BWC" sheetId="4" r:id="rId3"/>
-    <sheet name="150 mm BWC" sheetId="5" r:id="rId4"/>
-    <sheet name="150 mm TWC" sheetId="6" r:id="rId5"/>
-    <sheet name="200 mm TWC" sheetId="7" r:id="rId6"/>
+    <sheet name="110 mm Borewell Construction" sheetId="4" r:id="rId3"/>
+    <sheet name="150 mm Borewell Construction" sheetId="5" r:id="rId4"/>
+    <sheet name="150 mm Tubewell Construction" sheetId="6" r:id="rId5"/>
+    <sheet name="200 mm Tubewell Construction" sheetId="7" r:id="rId6"/>
     <sheet name="Submersible Pump Installation" sheetId="8" r:id="rId7"/>
     <sheet name="Compressor Pump Installation" sheetId="9" r:id="rId8"/>
   </sheets>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283C56C8-5101-4528-9234-DFAFA8B3C182}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8597B7-0160-4D8F-B8C8-FDE4C5B94C30}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1102,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BB96C7-B819-4358-9077-88E63A141CF4}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1363,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDC07DB-6CE0-44A7-A54C-721B3D36CA1E}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit 13-06-2025 14:30:43.09
</commit_message>
<xml_diff>
--- a/Templates.xlsx
+++ b/Templates.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\estimate-drafter\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D2BB97-1775-4D0E-95C8-EE274988FFC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="180" windowWidth="9860" windowHeight="7220" tabRatio="942" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="180" windowWidth="9860" windowHeight="7220" tabRatio="942" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="MWSS with Submersible Pump" sheetId="2" r:id="rId1"/>
@@ -22,7 +16,7 @@
     <sheet name="Submersible Pump Installation" sheetId="8" r:id="rId7"/>
     <sheet name="Compressor Pump Installation" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>Item Name</t>
   </si>
@@ -52,15 +46,6 @@
     <t>Providing and laying in position cement concrete of specified grade excluding the cost of centering and shuttering - All work up to plinth level: 1:2:4 )1 cement : 2 coarse sand : 4 graded stone aggregate 40 mm nominal size) (Code: 4.1.4)</t>
   </si>
   <si>
-    <t>40 mm dia UPVC pipe (Code: GWDMR103)</t>
-  </si>
-  <si>
-    <t>14 mm thick nylon rope (Code: GWDMR099)</t>
-  </si>
-  <si>
-    <t>40 mm SS Adapter (Code: GWDMR110)</t>
-  </si>
-  <si>
     <t>PVC Tank connector 40 mm (Code: GWDMR035)</t>
   </si>
   <si>
@@ -91,12 +76,6 @@
     <t>PVC End Cap 180 mm (DG) (Code: GWDMR005)</t>
   </si>
   <si>
-    <t>MS Casing pipe 450 mm dia, 6 mm thickness (Code: GWDMR117)</t>
-  </si>
-  <si>
-    <t>2 HP 18 Stage 120-40 m head single phase Submersible Pump including panel board (Code: GWDMR073)</t>
-  </si>
-  <si>
     <t>Flushing (Developing) Borewell (Code: GWDDR105)</t>
   </si>
   <si>
@@ -185,12 +164,36 @@
   </si>
   <si>
     <t>Providing and fixing G.I. pipes complete with G.I fittings including trenching and refilling etc. External work 25 mm dia nominal bore (18.12.3) (Code: GWDDR243)</t>
+  </si>
+  <si>
+    <t>Supply of Single Phase Submersible Pump 2 HP, Discharge 5200-10600 lph, Head 57-18m without Panel Board (Code: GWDMR149)</t>
+  </si>
+  <si>
+    <t>14 mm thick nylon rope (Code: GWDMR069)</t>
+  </si>
+  <si>
+    <t>40 mm dia UPVC pipe (Code: GWDMR073)</t>
+  </si>
+  <si>
+    <t>32 mm dia UPVC pipe (Code: GWDMR072)</t>
+  </si>
+  <si>
+    <t>20 mm dia HDPE pipe (DG) (8kg) (Code: GWDMR076)</t>
+  </si>
+  <si>
+    <t>40 mm SS Adapter (Code: GWDMR080)</t>
+  </si>
+  <si>
+    <t>Compressor pump 2 HP single phase (Code: GWDMR065)</t>
+  </si>
+  <si>
+    <t>MS Casing pipe 450 mm dia, 6 mm thickness (Code: GWDMR087)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -512,24 +515,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="255.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -542,7 +546,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -550,7 +554,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -558,7 +562,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -566,7 +570,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1">
         <v>85</v>
@@ -574,7 +578,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
         <v>85</v>
@@ -582,7 +586,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -590,7 +594,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -598,7 +602,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -606,7 +610,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -614,7 +618,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -622,7 +626,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -630,7 +634,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -646,7 +650,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -654,7 +658,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -662,7 +666,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -670,7 +674,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -678,7 +682,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>50</v>
@@ -686,7 +690,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>50</v>
@@ -694,7 +698,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
         <v>50</v>
@@ -702,7 +706,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>50</v>
@@ -718,7 +722,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>10</v>
@@ -747,17 +751,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="255.6328125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
@@ -771,7 +775,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -779,7 +783,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -787,7 +791,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -795,7 +799,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2">
         <v>15</v>
@@ -803,7 +807,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2">
         <v>50</v>
@@ -811,7 +815,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>60</v>
@@ -819,7 +823,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -827,7 +831,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -835,7 +839,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B10" s="2">
         <v>65</v>
@@ -843,7 +847,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <v>20</v>
@@ -851,7 +855,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -859,7 +863,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -867,7 +871,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
@@ -875,7 +879,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
@@ -883,7 +887,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -891,7 +895,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -907,7 +911,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
@@ -915,7 +919,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
@@ -923,7 +927,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
@@ -931,7 +935,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
@@ -939,7 +943,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2">
         <v>100</v>
@@ -947,7 +951,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2">
         <v>100</v>
@@ -955,7 +959,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2">
         <v>100</v>
@@ -963,7 +967,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2">
         <v>100</v>
@@ -979,7 +983,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>10</v>
@@ -1008,7 +1012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283C56C8-5101-4528-9234-DFAFA8B3C182}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1031,7 +1035,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1039,7 +1043,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -1047,7 +1051,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1060,15 +1064,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8597B7-0160-4D8F-B8C8-FDE4C5B94C30}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="255.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1080,7 +1087,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1088,7 +1095,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -1096,7 +1103,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1109,12 +1116,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BB96C7-B819-4358-9077-88E63A141CF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1132,7 +1139,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>150</v>
@@ -1140,7 +1147,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>120</v>
@@ -1148,7 +1155,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -1156,7 +1163,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1164,7 +1171,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1172,7 +1179,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -1185,12 +1192,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52A1A6B-7BA3-45B8-8EF7-73A16298341E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1208,7 +1215,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>150</v>
@@ -1216,7 +1223,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>120</v>
@@ -1224,7 +1231,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -1232,7 +1239,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1240,7 +1247,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1248,7 +1255,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -1261,15 +1268,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9A5F76-D8ED-42BD-9321-D6FD8EB33F52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="236.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1281,15 +1291,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>20</v>
+      <c r="A3" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1297,7 +1307,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1305,7 +1315,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B5">
         <v>85</v>
@@ -1313,7 +1323,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>85</v>
@@ -1321,7 +1331,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1329,7 +1339,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1337,7 +1347,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1345,7 +1355,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1353,7 +1363,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1361,7 +1371,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1373,15 +1383,18 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDC07DB-6CE0-44A7-A54C-721B3D36CA1E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="236.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1393,7 +1406,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1401,7 +1414,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1409,7 +1422,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1417,7 +1430,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -1425,7 +1438,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -1433,7 +1446,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B7">
         <v>60</v>
@@ -1441,7 +1454,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1449,7 +1462,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1457,7 +1470,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B10">
         <v>65</v>
@@ -1465,7 +1478,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -1473,7 +1486,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1481,7 +1494,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1489,7 +1502,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1497,7 +1510,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1505,7 +1518,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>1</v>

</xml_diff>

<commit_message>
Auto commit 13-06-2025 14:36:39.85
</commit_message>
<xml_diff>
--- a/Templates.xlsx
+++ b/Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="180" windowWidth="9860" windowHeight="7220" tabRatio="942" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-20" yWindow="180" windowWidth="9860" windowHeight="7220" tabRatio="942" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MWSS with Submersible Pump" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
   <si>
     <t>Item Name</t>
   </si>
@@ -56,15 +56,6 @@
   </si>
   <si>
     <t>PVC Ball valve 40 mm (Code: GWDMR042)</t>
-  </si>
-  <si>
-    <t>Compressor pump 2 HP single phase (Code: GWDMR095)</t>
-  </si>
-  <si>
-    <t>20 mm dia HDPE pipe (DG) (8kg) (Code: GWDMR106)</t>
-  </si>
-  <si>
-    <t>32 mm dia UPVC pipe (Code: GWDMR102)</t>
   </si>
   <si>
     <t>GI Bend 32 mm (Code: GWDMR052)</t>
@@ -515,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -527,7 +518,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,7 +537,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -554,7 +545,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -562,7 +553,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -570,7 +561,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1">
         <v>85</v>
@@ -578,7 +569,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>85</v>
@@ -586,7 +577,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -594,7 +585,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -602,7 +593,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -610,7 +601,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -618,7 +609,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -626,7 +617,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -634,7 +625,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -682,7 +673,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>50</v>
@@ -690,7 +681,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>50</v>
@@ -698,7 +689,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
         <v>50</v>
@@ -706,7 +697,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
         <v>50</v>
@@ -722,7 +713,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
         <v>10</v>
@@ -755,8 +746,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -775,7 +766,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -783,7 +774,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -791,7 +782,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -799,23 +790,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
+      <c r="A6" t="s">
+        <v>47</v>
       </c>
       <c r="B6" s="2">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
+      <c r="A7" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="2">
         <v>60</v>
@@ -823,7 +814,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -831,7 +822,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -839,7 +830,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2">
         <v>65</v>
@@ -847,7 +838,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2">
         <v>20</v>
@@ -855,7 +846,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -863,7 +854,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -871,7 +862,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
@@ -879,7 +870,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
@@ -887,7 +878,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -895,7 +886,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -943,7 +934,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2">
         <v>100</v>
@@ -951,7 +942,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2">
         <v>100</v>
@@ -959,7 +950,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2">
         <v>100</v>
@@ -967,7 +958,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2">
         <v>100</v>
@@ -983,7 +974,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" s="2">
         <v>10</v>
@@ -1035,7 +1026,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1043,7 +1034,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -1051,7 +1042,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1087,7 +1078,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1095,7 +1086,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -1103,7 +1094,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1139,7 +1130,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>150</v>
@@ -1147,7 +1138,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>120</v>
@@ -1155,7 +1146,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -1163,7 +1154,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1171,7 +1162,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1179,7 +1170,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -1196,7 +1187,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1215,7 +1206,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>150</v>
@@ -1223,7 +1214,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>120</v>
@@ -1231,7 +1222,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -1239,7 +1230,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1247,7 +1238,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1255,7 +1246,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -1291,7 +1282,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1299,7 +1290,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1307,7 +1298,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1315,7 +1306,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <v>85</v>
@@ -1323,7 +1314,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>85</v>
@@ -1331,7 +1322,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1339,7 +1330,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1347,7 +1338,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1355,7 +1346,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1363,7 +1354,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1371,7 +1362,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1388,7 +1379,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1406,15 +1397,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
+      <c r="A3" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1422,7 +1413,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1430,7 +1421,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -1438,7 +1429,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -1446,7 +1437,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>60</v>
@@ -1454,7 +1445,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1462,7 +1453,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1470,7 +1461,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>65</v>
@@ -1478,7 +1469,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -1486,7 +1477,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1494,7 +1485,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1502,7 +1493,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1510,7 +1501,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1518,7 +1509,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>1</v>

</xml_diff>